<commit_message>
Update with latest changes
</commit_message>
<xml_diff>
--- a/output/checks/dft2_type1_zz0_no_opinion.xlsx
+++ b/output/checks/dft2_type1_zz0_no_opinion.xlsx
@@ -382,7 +382,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>dft2_0b_s1_type1_no_op</t>
+          <t>dft2_z_s1_type1_no_op</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -395,14 +395,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>dft2_0b_s1_type1</t>
+          <t>dft2_z_s1_type1</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>dft2_a_s3_type1_no_op</t>
+          <t>dft2_z_s3_type1_no_op</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -415,7 +415,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>dft2_a_s3_type1</t>
+          <t>dft2_z_s3_type1</t>
         </is>
       </c>
     </row>

</xml_diff>